<commit_message>
BF: Remove (0, 0) as possible position in eyetracking demo
</commit_message>
<xml_diff>
--- a/psychopy/demos/builder/Feature Demos/eyetracking/trials_params.xlsx
+++ b/psychopy/demos/builder/Feature Demos/eyetracking/trials_params.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\GitHub\psychopy\psychopy\demos\builder\Feature Demos\eyetracking\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3B41532-8546-486E-B3C7-D62D1F1C90B0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91DC3FEB-0464-4DEA-8769-114CB067BF7F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="5">
   <si>
     <t>target_color</t>
   </si>
@@ -431,11 +431,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomLeft" activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -463,7 +463,7 @@
         <v>2</v>
       </c>
       <c r="C2">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -474,7 +474,7 @@
         <v>2</v>
       </c>
       <c r="C3">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -485,7 +485,7 @@
         <v>2</v>
       </c>
       <c r="C4">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -496,7 +496,7 @@
         <v>2</v>
       </c>
       <c r="C5">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -507,7 +507,7 @@
         <v>2</v>
       </c>
       <c r="C6">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -518,7 +518,7 @@
         <v>2</v>
       </c>
       <c r="C7">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -529,7 +529,7 @@
         <v>2</v>
       </c>
       <c r="C8">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -540,18 +540,18 @@
         <v>2</v>
       </c>
       <c r="C9">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B10" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C10">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -562,7 +562,7 @@
         <v>1</v>
       </c>
       <c r="C11">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -573,7 +573,7 @@
         <v>1</v>
       </c>
       <c r="C12">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -584,7 +584,7 @@
         <v>1</v>
       </c>
       <c r="C13">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -595,7 +595,7 @@
         <v>1</v>
       </c>
       <c r="C14">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -606,7 +606,7 @@
         <v>1</v>
       </c>
       <c r="C15">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -617,7 +617,7 @@
         <v>1</v>
       </c>
       <c r="C16">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -628,28 +628,6 @@
         <v>1</v>
       </c>
       <c r="C17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B18" t="s">
-        <v>1</v>
-      </c>
-      <c r="C18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B19" t="s">
-        <v>1</v>
-      </c>
-      <c r="C19">
         <v>0</v>
       </c>
     </row>

</xml_diff>